<commit_message>
update the test investment file
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Updated Assignments ISD\assignment_02\given_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e38070e6c41cb3e3/Desktop/Intermediate_software_development/Project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43D676BB-459D-41C1-84DA-85287089E7DE}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -246,6 +246,51 @@
   </si>
   <si>
     <t>date created exactly 10 years ago.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Account created &gt; 10 years ago</t>
+  </si>
+  <si>
+    <t>Account created exactly 10 years ago</t>
+  </si>
+  <si>
+    <t>Account created &lt; 10 years ago</t>
+  </si>
+  <si>
+    <t>59002635, 5550, 1200.00, date.today(), 2.00</t>
+  </si>
+  <si>
+    <t>59002635, 5550, 1200.00, date.today(), "invalid"</t>
+  </si>
+  <si>
+    <t>59002635, 5550, 1200.00, date.today() - timedelta(days=10*365.26)</t>
+  </si>
+  <si>
+    <t>59002635, 5550, 1200.00, date.today() - timedelta(days=10*365.25)</t>
+  </si>
+  <si>
+    <t>Account number: 59002635, Client number: 5550, Balance: 1200.00, Date created: today, Management fee: 2.00</t>
+  </si>
+  <si>
+    <t>Management fee is set to 2.55</t>
+  </si>
+  <si>
+    <t>Service charge equals BASE_SERVICE_CHARGE</t>
+  </si>
+  <si>
+    <t>Service charge equals BASE_SERVICE_CHARGE + 2.00</t>
+  </si>
+  <si>
+    <t>String includes "Management Fee: Waived"</t>
+  </si>
+  <si>
+    <t>String includes "Management Fee: $2.00"</t>
+  </si>
+  <si>
+    <t>Sukhtab Singh Warya</t>
   </si>
 </sst>
 </file>
@@ -552,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -571,14 +616,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -590,9 +629,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -607,6 +643,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1150,55 +1202,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
-  <dimension ref="B1:G34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="49.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1218,125 +1272,174 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11">
+    <row r="7" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+      <c r="E7" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="21"/>
+      <c r="B8" s="24">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11">
+      <c r="E8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11">
+      <c r="E9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11">
+      <c r="E10" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
+      <c r="E11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="21"/>
+      <c r="B12" s="24">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+      <c r="E12" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22">
         <v>7</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+      <c r="E13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="10">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="10">
         <v>9</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="3">
         <v>10</v>
       </c>
@@ -1346,8 +1449,8 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="10">
         <v>11</v>
       </c>
       <c r="C17" s="4"/>
@@ -1356,8 +1459,8 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="10">
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
@@ -1366,8 +1469,8 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="10">
         <v>13</v>
       </c>
       <c r="C19" s="4"/>
@@ -1376,7 +1479,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1386,8 +1489,8 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="10">
         <v>15</v>
       </c>
       <c r="C21" s="4"/>
@@ -1396,8 +1499,8 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="10">
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
@@ -1406,8 +1509,8 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="10">
         <v>17</v>
       </c>
       <c r="C23" s="4"/>
@@ -1416,7 +1519,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3">
         <v>18</v>
       </c>
@@ -1426,8 +1529,8 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="10">
         <v>19</v>
       </c>
       <c r="C25" s="4"/>
@@ -1436,8 +1539,8 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="10">
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
@@ -1446,8 +1549,8 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="10">
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
@@ -1456,7 +1559,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="3">
         <v>22</v>
       </c>
@@ -1466,8 +1569,8 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="10">
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
@@ -1476,8 +1579,8 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="10">
         <v>24</v>
       </c>
       <c r="C30" s="4"/>
@@ -1486,8 +1589,8 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
+    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="10">
         <v>25</v>
       </c>
       <c r="C31" s="4"/>
@@ -1496,7 +1599,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="3">
         <v>26</v>
       </c>
@@ -1506,15 +1609,15 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>